<commit_message>
updated Box Office Mojo Data
</commit_message>
<xml_diff>
--- a/Box Office Mojo Data/2014 Box Office.xlsx
+++ b/Box Office Mojo Data/2014 Box Office.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gkchan\Documents\Project\Project-1-DS-Viz-Bootcamp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gkchan\Documents\Project\Project-1-DS-Viz-Bootcamp\Box Office Mojo Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Rank</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Fox</t>
+  </si>
+  <si>
+    <t>Big Hero 6</t>
   </si>
 </sst>
 </file>
@@ -450,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,6 +756,35 @@
         <v>43382</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1">
+        <v>222527828</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3773</v>
+      </c>
+      <c r="F11" s="1">
+        <v>56215889</v>
+      </c>
+      <c r="G11" s="2">
+        <v>3761</v>
+      </c>
+      <c r="H11" s="3">
+        <v>43411</v>
+      </c>
+      <c r="I11" s="3">
+        <v>43248</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>